<commit_message>
5.1.2012 update Best20Places.xlsx toa do Binh Quoi
</commit_message>
<xml_diff>
--- a/Best20Places.xlsx
+++ b/Best20Places.xlsx
@@ -1893,11 +1893,11 @@
       </c>
       <c r="D2" t="str">
         <f ca="1">RANDBETWEEN(1965, 2000)&amp;"-1-1"</f>
-        <v>1965-1-1</v>
+        <v>1968-1-1</v>
       </c>
       <c r="E2">
         <f ca="1">RANDBETWEEN(0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1910,7 +1910,7 @@
       </c>
       <c r="D3" t="str">
         <f t="shared" ref="D3:D66" ca="1" si="1">RANDBETWEEN(1965, 2000)&amp;"-1-1"</f>
-        <v>1971-1-1</v>
+        <v>1996-1-1</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E66" ca="1" si="2">RANDBETWEEN(0,1)</f>
@@ -1927,7 +1927,7 @@
       </c>
       <c r="D4" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1984-1-1</v>
+        <v>1979-1-1</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="2"/>
@@ -1944,7 +1944,7 @@
       </c>
       <c r="D5" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1983-1-1</v>
+        <v>1982-1-1</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="2"/>
@@ -1961,11 +1961,11 @@
       </c>
       <c r="D6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1983-1-1</v>
+        <v>1979-1-1</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1978,7 +1978,7 @@
       </c>
       <c r="D7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1995-1-1</v>
+        <v>1980-1-1</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="2"/>
@@ -1995,7 +1995,7 @@
       </c>
       <c r="D8" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1968-1-1</v>
+        <v>1971-1-1</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="2"/>
@@ -2012,7 +2012,7 @@
       </c>
       <c r="D9" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2000-1-1</v>
+        <v>1980-1-1</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="2"/>
@@ -2029,7 +2029,7 @@
       </c>
       <c r="D10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1989-1-1</v>
+        <v>1983-1-1</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="2"/>
@@ -2046,11 +2046,11 @@
       </c>
       <c r="D11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1966-1-1</v>
+        <v>1987-1-1</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2063,11 +2063,11 @@
       </c>
       <c r="D12" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1986-1-1</v>
+        <v>1993-1-1</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2080,11 +2080,11 @@
       </c>
       <c r="D13" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2000-1-1</v>
+        <v>1970-1-1</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2097,11 +2097,11 @@
       </c>
       <c r="D14" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1968-1-1</v>
+        <v>1969-1-1</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2114,7 +2114,7 @@
       </c>
       <c r="D15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1967-1-1</v>
+        <v>1999-1-1</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="2"/>
@@ -2131,11 +2131,11 @@
       </c>
       <c r="D16" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1994-1-1</v>
+        <v>1978-1-1</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2148,11 +2148,11 @@
       </c>
       <c r="D17" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2000-1-1</v>
+        <v>1990-1-1</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2165,7 +2165,7 @@
       </c>
       <c r="D18" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1977-1-1</v>
+        <v>1987-1-1</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="2"/>
@@ -2182,7 +2182,7 @@
       </c>
       <c r="D19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1973-1-1</v>
+        <v>1987-1-1</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="2"/>
@@ -2199,7 +2199,7 @@
       </c>
       <c r="D20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1984-1-1</v>
+        <v>1967-1-1</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="2"/>
@@ -2216,11 +2216,11 @@
       </c>
       <c r="D21" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1999-1-1</v>
+        <v>1975-1-1</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2233,7 +2233,7 @@
       </c>
       <c r="D22" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1977-1-1</v>
+        <v>1969-1-1</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="2"/>
@@ -2250,7 +2250,7 @@
       </c>
       <c r="D23" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1968-1-1</v>
+        <v>1992-1-1</v>
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="2"/>
@@ -2267,7 +2267,7 @@
       </c>
       <c r="D24" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2000-1-1</v>
+        <v>1987-1-1</v>
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="2"/>
@@ -2284,11 +2284,11 @@
       </c>
       <c r="D25" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1997-1-1</v>
+        <v>1994-1-1</v>
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -2301,11 +2301,11 @@
       </c>
       <c r="D26" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1999-1-1</v>
+        <v>1987-1-1</v>
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -2318,7 +2318,7 @@
       </c>
       <c r="D27" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1983-1-1</v>
+        <v>1978-1-1</v>
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="2"/>
@@ -2352,7 +2352,7 @@
       </c>
       <c r="D29" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1970-1-1</v>
+        <v>1981-1-1</v>
       </c>
       <c r="E29">
         <f t="shared" ca="1" si="2"/>
@@ -2369,11 +2369,11 @@
       </c>
       <c r="D30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2000-1-1</v>
+        <v>1974-1-1</v>
       </c>
       <c r="E30">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -2386,11 +2386,11 @@
       </c>
       <c r="D31" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1999-1-1</v>
+        <v>1972-1-1</v>
       </c>
       <c r="E31">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -2403,11 +2403,11 @@
       </c>
       <c r="D32" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1966-1-1</v>
+        <v>1975-1-1</v>
       </c>
       <c r="E32">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -2420,11 +2420,11 @@
       </c>
       <c r="D33" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1970-1-1</v>
+        <v>1967-1-1</v>
       </c>
       <c r="E33">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -2437,7 +2437,7 @@
       </c>
       <c r="D34" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1991-1-1</v>
+        <v>1981-1-1</v>
       </c>
       <c r="E34">
         <f t="shared" ca="1" si="2"/>
@@ -2454,11 +2454,11 @@
       </c>
       <c r="D35" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1991-1-1</v>
+        <v>1997-1-1</v>
       </c>
       <c r="E35">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -2471,11 +2471,11 @@
       </c>
       <c r="D36" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1987-1-1</v>
+        <v>1972-1-1</v>
       </c>
       <c r="E36">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -2488,7 +2488,7 @@
       </c>
       <c r="D37" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1994-1-1</v>
+        <v>1978-1-1</v>
       </c>
       <c r="E37">
         <f t="shared" ca="1" si="2"/>
@@ -2505,7 +2505,7 @@
       </c>
       <c r="D38" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1990-1-1</v>
+        <v>1991-1-1</v>
       </c>
       <c r="E38">
         <f t="shared" ca="1" si="2"/>
@@ -2522,7 +2522,7 @@
       </c>
       <c r="D39" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1995-1-1</v>
+        <v>1973-1-1</v>
       </c>
       <c r="E39">
         <f t="shared" ca="1" si="2"/>
@@ -2539,7 +2539,7 @@
       </c>
       <c r="D40" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1998-1-1</v>
+        <v>1986-1-1</v>
       </c>
       <c r="E40">
         <f t="shared" ca="1" si="2"/>
@@ -2556,11 +2556,11 @@
       </c>
       <c r="D41" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1998-1-1</v>
+        <v>1989-1-1</v>
       </c>
       <c r="E41">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -2573,11 +2573,11 @@
       </c>
       <c r="D42" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1987-1-1</v>
+        <v>1984-1-1</v>
       </c>
       <c r="E42">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -2590,11 +2590,11 @@
       </c>
       <c r="D43" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1965-1-1</v>
+        <v>1976-1-1</v>
       </c>
       <c r="E43">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -2607,11 +2607,11 @@
       </c>
       <c r="D44" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1977-1-1</v>
+        <v>1965-1-1</v>
       </c>
       <c r="E44">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -2624,7 +2624,7 @@
       </c>
       <c r="D45" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1987-1-1</v>
+        <v>1971-1-1</v>
       </c>
       <c r="E45">
         <f t="shared" ca="1" si="2"/>
@@ -2641,11 +2641,11 @@
       </c>
       <c r="D46" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1979-1-1</v>
+        <v>1967-1-1</v>
       </c>
       <c r="E46">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -2658,11 +2658,11 @@
       </c>
       <c r="D47" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1989-1-1</v>
+        <v>1967-1-1</v>
       </c>
       <c r="E47">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -2675,7 +2675,7 @@
       </c>
       <c r="D48" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1984-1-1</v>
+        <v>1982-1-1</v>
       </c>
       <c r="E48">
         <f t="shared" ca="1" si="2"/>
@@ -2692,11 +2692,11 @@
       </c>
       <c r="D49" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2000-1-1</v>
+        <v>1984-1-1</v>
       </c>
       <c r="E49">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -2709,11 +2709,11 @@
       </c>
       <c r="D50" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1975-1-1</v>
+        <v>1985-1-1</v>
       </c>
       <c r="E50">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -2726,7 +2726,7 @@
       </c>
       <c r="D51" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1975-1-1</v>
+        <v>1998-1-1</v>
       </c>
       <c r="E51">
         <f t="shared" ca="1" si="2"/>
@@ -2743,11 +2743,11 @@
       </c>
       <c r="D52" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1973-1-1</v>
+        <v>1990-1-1</v>
       </c>
       <c r="E52">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -2760,7 +2760,7 @@
       </c>
       <c r="D53" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1986-1-1</v>
+        <v>1985-1-1</v>
       </c>
       <c r="E53">
         <f t="shared" ca="1" si="2"/>
@@ -2777,11 +2777,11 @@
       </c>
       <c r="D54" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1992-1-1</v>
+        <v>1969-1-1</v>
       </c>
       <c r="E54">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -2794,7 +2794,7 @@
       </c>
       <c r="D55" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1989-1-1</v>
+        <v>1986-1-1</v>
       </c>
       <c r="E55">
         <f t="shared" ca="1" si="2"/>
@@ -2811,11 +2811,11 @@
       </c>
       <c r="D56" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1986-1-1</v>
+        <v>1998-1-1</v>
       </c>
       <c r="E56">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -2828,11 +2828,11 @@
       </c>
       <c r="D57" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1995-1-1</v>
+        <v>1997-1-1</v>
       </c>
       <c r="E57">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -2845,7 +2845,7 @@
       </c>
       <c r="D58" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1999-1-1</v>
+        <v>1986-1-1</v>
       </c>
       <c r="E58">
         <f t="shared" ca="1" si="2"/>
@@ -2862,7 +2862,7 @@
       </c>
       <c r="D59" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1978-1-1</v>
+        <v>1972-1-1</v>
       </c>
       <c r="E59">
         <f t="shared" ca="1" si="2"/>
@@ -2879,11 +2879,11 @@
       </c>
       <c r="D60" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1969-1-1</v>
+        <v>1965-1-1</v>
       </c>
       <c r="E60">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -2896,7 +2896,7 @@
       </c>
       <c r="D61" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1969-1-1</v>
+        <v>1985-1-1</v>
       </c>
       <c r="E61">
         <f t="shared" ca="1" si="2"/>
@@ -2913,7 +2913,7 @@
       </c>
       <c r="D62" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1998-1-1</v>
+        <v>1974-1-1</v>
       </c>
       <c r="E62">
         <f t="shared" ca="1" si="2"/>
@@ -2930,11 +2930,11 @@
       </c>
       <c r="D63" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1979-1-1</v>
+        <v>1982-1-1</v>
       </c>
       <c r="E63">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -2951,7 +2951,7 @@
       </c>
       <c r="E64">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -2964,11 +2964,11 @@
       </c>
       <c r="D65" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1972-1-1</v>
+        <v>1992-1-1</v>
       </c>
       <c r="E65">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -2981,7 +2981,7 @@
       </c>
       <c r="D66" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>1999-1-1</v>
+        <v>1970-1-1</v>
       </c>
       <c r="E66">
         <f t="shared" ca="1" si="2"/>
@@ -2998,11 +2998,11 @@
       </c>
       <c r="D67" t="str">
         <f t="shared" ref="D67:D100" ca="1" si="4">RANDBETWEEN(1965, 2000)&amp;"-1-1"</f>
-        <v>1993-1-1</v>
+        <v>1996-1-1</v>
       </c>
       <c r="E67">
         <f t="shared" ref="E67:E100" ca="1" si="5">RANDBETWEEN(0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -3015,7 +3015,7 @@
       </c>
       <c r="D68" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1969-1-1</v>
+        <v>1994-1-1</v>
       </c>
       <c r="E68">
         <f t="shared" ca="1" si="5"/>
@@ -3032,11 +3032,11 @@
       </c>
       <c r="D69" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1983-1-1</v>
+        <v>1997-1-1</v>
       </c>
       <c r="E69">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -3049,7 +3049,7 @@
       </c>
       <c r="D70" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1968-1-1</v>
+        <v>1976-1-1</v>
       </c>
       <c r="E70">
         <f t="shared" ca="1" si="5"/>
@@ -3066,11 +3066,11 @@
       </c>
       <c r="D71" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1982-1-1</v>
+        <v>1984-1-1</v>
       </c>
       <c r="E71">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -3083,11 +3083,11 @@
       </c>
       <c r="D72" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1983-1-1</v>
+        <v>2000-1-1</v>
       </c>
       <c r="E72">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -3100,11 +3100,11 @@
       </c>
       <c r="D73" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1983-1-1</v>
+        <v>1982-1-1</v>
       </c>
       <c r="E73">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -3117,7 +3117,7 @@
       </c>
       <c r="D74" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1995-1-1</v>
+        <v>1990-1-1</v>
       </c>
       <c r="E74">
         <f t="shared" ca="1" si="5"/>
@@ -3134,11 +3134,11 @@
       </c>
       <c r="D75" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1987-1-1</v>
+        <v>1999-1-1</v>
       </c>
       <c r="E75">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -3151,7 +3151,7 @@
       </c>
       <c r="D76" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1996-1-1</v>
+        <v>1982-1-1</v>
       </c>
       <c r="E76">
         <f t="shared" ca="1" si="5"/>
@@ -3168,11 +3168,11 @@
       </c>
       <c r="D77" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1989-1-1</v>
+        <v>1976-1-1</v>
       </c>
       <c r="E77">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -3185,7 +3185,7 @@
       </c>
       <c r="D78" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1985-1-1</v>
+        <v>1990-1-1</v>
       </c>
       <c r="E78">
         <f t="shared" ca="1" si="5"/>
@@ -3202,7 +3202,7 @@
       </c>
       <c r="D79" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1994-1-1</v>
+        <v>1989-1-1</v>
       </c>
       <c r="E79">
         <f t="shared" ca="1" si="5"/>
@@ -3219,11 +3219,11 @@
       </c>
       <c r="D80" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1984-1-1</v>
+        <v>1978-1-1</v>
       </c>
       <c r="E80">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -3236,7 +3236,7 @@
       </c>
       <c r="D81" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1987-1-1</v>
+        <v>1975-1-1</v>
       </c>
       <c r="E81">
         <f t="shared" ca="1" si="5"/>
@@ -3253,7 +3253,7 @@
       </c>
       <c r="D82" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1977-1-1</v>
+        <v>1972-1-1</v>
       </c>
       <c r="E82">
         <f t="shared" ca="1" si="5"/>
@@ -3270,7 +3270,7 @@
       </c>
       <c r="D83" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1980-1-1</v>
+        <v>1965-1-1</v>
       </c>
       <c r="E83">
         <f t="shared" ca="1" si="5"/>
@@ -3287,11 +3287,11 @@
       </c>
       <c r="D84" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1965-1-1</v>
+        <v>1993-1-1</v>
       </c>
       <c r="E84">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -3304,7 +3304,7 @@
       </c>
       <c r="D85" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1983-1-1</v>
+        <v>2000-1-1</v>
       </c>
       <c r="E85">
         <f t="shared" ca="1" si="5"/>
@@ -3321,11 +3321,11 @@
       </c>
       <c r="D86" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1989-1-1</v>
+        <v>1990-1-1</v>
       </c>
       <c r="E86">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -3338,11 +3338,11 @@
       </c>
       <c r="D87" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1978-1-1</v>
+        <v>1988-1-1</v>
       </c>
       <c r="E87">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -3355,11 +3355,11 @@
       </c>
       <c r="D88" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1967-1-1</v>
+        <v>1971-1-1</v>
       </c>
       <c r="E88">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -3372,7 +3372,7 @@
       </c>
       <c r="D89" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1974-1-1</v>
+        <v>1980-1-1</v>
       </c>
       <c r="E89">
         <f t="shared" ca="1" si="5"/>
@@ -3389,11 +3389,11 @@
       </c>
       <c r="D90" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1992-1-1</v>
+        <v>1978-1-1</v>
       </c>
       <c r="E90">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -3406,7 +3406,7 @@
       </c>
       <c r="D91" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1996-1-1</v>
+        <v>1978-1-1</v>
       </c>
       <c r="E91">
         <f t="shared" ca="1" si="5"/>
@@ -3423,7 +3423,7 @@
       </c>
       <c r="D92" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1967-1-1</v>
+        <v>2000-1-1</v>
       </c>
       <c r="E92">
         <f t="shared" ca="1" si="5"/>
@@ -3440,11 +3440,11 @@
       </c>
       <c r="D93" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1985-1-1</v>
+        <v>1999-1-1</v>
       </c>
       <c r="E93">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -3457,7 +3457,7 @@
       </c>
       <c r="D94" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1965-1-1</v>
+        <v>1972-1-1</v>
       </c>
       <c r="E94">
         <f t="shared" ca="1" si="5"/>
@@ -3474,7 +3474,7 @@
       </c>
       <c r="D95" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1999-1-1</v>
+        <v>1991-1-1</v>
       </c>
       <c r="E95">
         <f t="shared" ca="1" si="5"/>
@@ -3491,11 +3491,11 @@
       </c>
       <c r="D96" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1968-1-1</v>
+        <v>1994-1-1</v>
       </c>
       <c r="E96">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -3508,7 +3508,7 @@
       </c>
       <c r="D97" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1974-1-1</v>
+        <v>1997-1-1</v>
       </c>
       <c r="E97">
         <f t="shared" ca="1" si="5"/>
@@ -3525,7 +3525,7 @@
       </c>
       <c r="D98" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1988-1-1</v>
+        <v>1967-1-1</v>
       </c>
       <c r="E98">
         <f t="shared" ca="1" si="5"/>
@@ -3542,7 +3542,7 @@
       </c>
       <c r="D99" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1980-1-1</v>
+        <v>1993-1-1</v>
       </c>
       <c r="E99">
         <f t="shared" ca="1" si="5"/>
@@ -3559,11 +3559,11 @@
       </c>
       <c r="D100" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1992-1-1</v>
+        <v>1974-1-1</v>
       </c>
       <c r="E100">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3933,8 +3933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5122,10 +5122,10 @@
         <v>258</v>
       </c>
       <c r="E19">
-        <v>10.832378</v>
+        <v>10.833758</v>
       </c>
       <c r="F19">
-        <v>106.73774299999999</v>
+        <v>106.743252</v>
       </c>
       <c r="G19" s="6" t="s">
         <v>199</v>

</xml_diff>